<commit_message>
update data add talent exclusive
</commit_message>
<xml_diff>
--- a/data/talents.xlsx
+++ b/data/talents.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84694\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\lifeRestart\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F982F1D-BBE1-4E1F-8701-16A3046716A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEB8545-5A7E-4942-9361-B0347271C9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="490" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="talents" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <author>84694</author>
   </authors>
   <commentList>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{F13F5F22-BDEB-4992-9B66-ED7757A7DEBD}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{F13F5F22-BDEB-4992-9B66-ED7757A7DEBD}">
       <text>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{CFC59F7C-A7E9-4DCF-A179-85D48981585F}">
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{CFC59F7C-A7E9-4DCF-A179-85D48981585F}">
       <text>
         <r>
           <rPr>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="397">
   <si>
     <t>序号</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -822,10 +822,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>你的家人不会发生车祸</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>老司机</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1492,6 +1488,66 @@
   </si>
   <si>
     <t>你不吃洋快餐</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>互斥天赋</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>exclusive[]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不想罢了</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你不会上清华大学</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>挑衅</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你喜欢没事找事</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你和家人不会发生车祸</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你喜欢旅游</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你比较自恋</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>旅行者</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>水仙</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>缺一门</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>无效果</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你可能听到一些绝密消息</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>异界来客</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1590,7 +1646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1605,6 +1661,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1887,103 +1952,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K120"/>
+  <dimension ref="A1:N120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F108" sqref="F108"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.44140625" defaultRowHeight="39.6" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="25.4140625" defaultRowHeight="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" style="1"/>
-    <col min="2" max="2" width="27.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.4140625" style="1"/>
+    <col min="2" max="2" width="27.4140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="33" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
-    <col min="7" max="11" width="13.5546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.88671875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5546875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="13" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13" style="6" customWidth="1"/>
+    <col min="7" max="7" width="20.9140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.08203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" style="1" customWidth="1"/>
+    <col min="10" max="14" width="13.58203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.4140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.9140625" style="1" customWidth="1"/>
     <col min="18" max="18" width="10" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="25.44140625" style="1"/>
+    <col min="19" max="19" width="8.9140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.58203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="25.4140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="3" customFormat="1" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1993,11 +2078,11 @@
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2007,11 +2092,11 @@
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -2021,11 +2106,20 @@
       <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="D5" s="6">
+        <v>1004</v>
+      </c>
       <c r="E5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1024</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1025</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -2035,11 +2129,20 @@
       <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="D6" s="6">
+        <v>1003</v>
+      </c>
       <c r="E6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1024</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1025</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -2049,11 +2152,12 @@
       <c r="C7" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="6"/>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -2063,14 +2167,15 @@
       <c r="C8" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="6"/>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -2080,14 +2185,15 @@
       <c r="C9" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="6"/>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -2097,14 +2203,15 @@
       <c r="C10" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
+      <c r="D10" s="6"/>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
         <v>-3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -2114,14 +2221,15 @@
       <c r="C11" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="6"/>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -2131,11 +2239,12 @@
       <c r="C12" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E12" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="6"/>
+      <c r="H12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -2145,11 +2254,12 @@
       <c r="C13" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="6"/>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -2159,11 +2269,20 @@
       <c r="C14" s="1" t="s">
         <v>144</v>
       </c>
+      <c r="D14" s="6">
+        <v>1013</v>
+      </c>
       <c r="E14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1014</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1010</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -2173,11 +2292,20 @@
       <c r="C15" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="D15" s="6">
+        <v>1010</v>
+      </c>
       <c r="E15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1012</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -2187,14 +2315,23 @@
       <c r="C16" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="D16" s="6">
+        <v>1010</v>
+      </c>
       <c r="E16" s="1">
-        <v>2</v>
+        <v>1012</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1013</v>
       </c>
       <c r="H16" s="1">
+        <v>2</v>
+      </c>
+      <c r="K16" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -2204,11 +2341,11 @@
       <c r="C17" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -2218,11 +2355,11 @@
       <c r="C18" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -2232,31 +2369,22 @@
       <c r="C19" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E20" s="1">
-        <v>2</v>
-      </c>
-      <c r="G20" s="1">
-        <v>1</v>
-      </c>
       <c r="H20" s="1">
-        <v>1</v>
-      </c>
-      <c r="I20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J20" s="1">
         <v>1</v>
@@ -2264,8 +2392,17 @@
       <c r="K20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L20" s="1">
+        <v>1</v>
+      </c>
+      <c r="M20" s="1">
+        <v>1</v>
+      </c>
+      <c r="N20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -2273,16 +2410,16 @@
         <v>164</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="E21" s="1">
-        <v>2</v>
-      </c>
-      <c r="F21" s="1">
+        <v>261</v>
+      </c>
+      <c r="H21" s="1">
+        <v>2</v>
+      </c>
+      <c r="I21" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -2292,14 +2429,14 @@
       <c r="C22" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E22" s="1">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="L22" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
@@ -2309,17 +2446,17 @@
       <c r="C23" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1">
-        <v>2</v>
-      </c>
-      <c r="J23" s="1">
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>2</v>
+      </c>
+      <c r="M23" s="1">
         <v>-2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -2329,11 +2466,11 @@
       <c r="C24" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E24" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
@@ -2343,26 +2480,26 @@
       <c r="C25" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E25" s="1">
+      <c r="H25" s="1">
         <v>3</v>
       </c>
-      <c r="G25" s="1">
-        <v>2</v>
-      </c>
-      <c r="H25" s="1">
-        <v>2</v>
-      </c>
-      <c r="I25" s="1">
-        <v>2</v>
-      </c>
       <c r="J25" s="1">
         <v>2</v>
       </c>
       <c r="K25" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L25" s="1">
+        <v>2</v>
+      </c>
+      <c r="M25" s="1">
+        <v>2</v>
+      </c>
+      <c r="N25" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
@@ -2372,11 +2509,20 @@
       <c r="C26" s="1" t="s">
         <v>174</v>
       </c>
+      <c r="D26" s="6">
+        <v>1003</v>
+      </c>
       <c r="E26" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1004</v>
+      </c>
+      <c r="F26" s="6">
+        <v>1025</v>
+      </c>
+      <c r="H26" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
@@ -2386,11 +2532,20 @@
       <c r="C27" s="1" t="s">
         <v>176</v>
       </c>
+      <c r="D27" s="6">
+        <v>1003</v>
+      </c>
       <c r="E27" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1024</v>
+      </c>
+      <c r="F27" s="6">
+        <v>1004</v>
+      </c>
+      <c r="H27" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
@@ -2400,11 +2555,11 @@
       <c r="C28" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -2414,11 +2569,11 @@
       <c r="C29" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>42</v>
       </c>
@@ -2428,11 +2583,11 @@
       <c r="C30" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E30" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>43</v>
       </c>
@@ -2442,11 +2597,11 @@
       <c r="C31" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -2456,11 +2611,11 @@
       <c r="C32" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>45</v>
       </c>
@@ -2470,14 +2625,14 @@
       <c r="C33" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E33" s="1">
-        <v>0</v>
-      </c>
-      <c r="J33" s="1">
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1">
         <v>-2</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -2487,17 +2642,8 @@
       <c r="C34" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E34" s="1">
-        <v>0</v>
-      </c>
-      <c r="G34" s="1">
-        <v>-1</v>
-      </c>
       <c r="H34" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I34" s="1">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J34" s="1">
         <v>-1</v>
@@ -2505,8 +2651,17 @@
       <c r="K34" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L34" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M34" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N34" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>47</v>
       </c>
@@ -2516,14 +2671,14 @@
       <c r="C35" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E35" s="1">
-        <v>0</v>
-      </c>
-      <c r="J35" s="1">
+      <c r="H35" s="1">
+        <v>0</v>
+      </c>
+      <c r="M35" s="1">
         <v>-10</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>48</v>
       </c>
@@ -2533,14 +2688,14 @@
       <c r="C36" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E36" s="1">
-        <v>0</v>
-      </c>
       <c r="H36" s="1">
+        <v>0</v>
+      </c>
+      <c r="K36" s="1">
         <v>-2</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>49</v>
       </c>
@@ -2550,14 +2705,14 @@
       <c r="C37" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E37" s="1">
-        <v>0</v>
-      </c>
-      <c r="K37" s="1">
+      <c r="H37" s="1">
+        <v>0</v>
+      </c>
+      <c r="N37" s="1">
         <v>-2</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>50</v>
       </c>
@@ -2567,14 +2722,14 @@
       <c r="C38" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E38" s="1">
-        <v>0</v>
-      </c>
-      <c r="K38" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+      <c r="N38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>51</v>
       </c>
@@ -2584,11 +2739,11 @@
       <c r="C39" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E39" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>52</v>
       </c>
@@ -2598,11 +2753,11 @@
       <c r="C40" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E40" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>53</v>
       </c>
@@ -2612,11 +2767,11 @@
       <c r="C41" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E41" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>54</v>
       </c>
@@ -2626,11 +2781,11 @@
       <c r="C42" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E42" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>55</v>
       </c>
@@ -2640,11 +2795,11 @@
       <c r="C43" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E43" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>56</v>
       </c>
@@ -2654,990 +2809,984 @@
       <c r="C44" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E44" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E45" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>388</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E46" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E47" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E48" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E49" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E50" s="1">
+        <v>220</v>
+      </c>
+      <c r="H50" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="E51" s="1">
-        <v>0</v>
+        <v>231</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>280</v>
       </c>
       <c r="H51" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K51" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E52" s="1">
-        <v>0</v>
-      </c>
-      <c r="K52" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="H52" s="1">
+        <v>0</v>
+      </c>
+      <c r="N52" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E53" s="1">
-        <v>0</v>
-      </c>
-      <c r="G53" s="1">
-        <v>1</v>
-      </c>
-      <c r="K53" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G53" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="H53" s="1">
+        <v>0</v>
+      </c>
+      <c r="J53" s="1">
+        <v>1</v>
+      </c>
+      <c r="N53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E54" s="1">
-        <v>0</v>
-      </c>
-      <c r="G54" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G54" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="H54" s="1">
+        <v>0</v>
+      </c>
+      <c r="J54" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="E55" s="1">
-        <v>0</v>
-      </c>
-      <c r="G55" s="1">
+      <c r="G55" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="H55" s="1">
+        <v>0</v>
+      </c>
+      <c r="J55" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E56" s="1">
-        <v>1</v>
-      </c>
-      <c r="J56" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G56" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="H56" s="1">
+        <v>1</v>
+      </c>
+      <c r="M56" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="E57" s="1">
-        <v>0</v>
-      </c>
-      <c r="I57" s="1">
+      <c r="G57" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="H57" s="1">
+        <v>0</v>
+      </c>
+      <c r="L57" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="E58" s="1">
-        <v>1</v>
-      </c>
-      <c r="K58" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G58" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="H58" s="1">
+        <v>1</v>
+      </c>
+      <c r="N58" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="E59" s="1">
-        <v>1</v>
-      </c>
-      <c r="I59" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G59" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="H59" s="1">
+        <v>1</v>
+      </c>
+      <c r="L59" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E60" s="1">
-        <v>0</v>
+      <c r="G60" s="1" t="s">
+        <v>287</v>
       </c>
       <c r="H60" s="1">
+        <v>0</v>
+      </c>
+      <c r="K60" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E61" s="1">
-        <v>0</v>
+      <c r="G61" s="1" t="s">
+        <v>288</v>
       </c>
       <c r="H61" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E62" s="1">
-        <v>1</v>
-      </c>
-      <c r="K62" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G62" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="H62" s="1">
+        <v>1</v>
+      </c>
+      <c r="N62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="E63" s="1">
-        <v>1</v>
-      </c>
-      <c r="I63" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G63" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H63" s="1">
+        <v>1</v>
+      </c>
+      <c r="L63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="E64" s="1">
-        <v>0</v>
-      </c>
-      <c r="G64" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G64" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="H64" s="1">
+        <v>0</v>
+      </c>
+      <c r="J64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="E65" s="1">
-        <v>0</v>
-      </c>
-      <c r="F65" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+      <c r="H65" s="1">
+        <v>0</v>
+      </c>
+      <c r="I65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E66" s="1">
+        <v>260</v>
+      </c>
+      <c r="H66" s="1">
         <v>3</v>
       </c>
-      <c r="F66" s="1">
+      <c r="I66" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="E67" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+      <c r="H67" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="E68" s="1">
-        <v>0</v>
+        <v>268</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="H68" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K68" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="E69" s="1">
-        <v>1</v>
-      </c>
-      <c r="G69" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G69" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="H69" s="1">
+        <v>1</v>
+      </c>
+      <c r="J69" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="E70" s="1">
-        <v>0</v>
-      </c>
-      <c r="J70" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="H70" s="1">
+        <v>0</v>
+      </c>
+      <c r="M70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="E71" s="1">
-        <v>0</v>
+      <c r="G71" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="H71" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K71" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="E72" s="1">
-        <v>0</v>
-      </c>
-      <c r="G72" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G72" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="H72" s="1">
+        <v>0</v>
+      </c>
+      <c r="J72" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="E73" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H73" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E74" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+      <c r="H74" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="E75" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H75" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="G76" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E76" s="1">
-        <v>0</v>
-      </c>
-      <c r="G76" s="1">
+      <c r="H76" s="1">
+        <v>1</v>
+      </c>
+      <c r="J76" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="E77" s="1">
-        <v>0</v>
-      </c>
-      <c r="I77" s="1">
+      <c r="H77" s="1">
+        <v>0</v>
+      </c>
+      <c r="L77" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="D78" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="E78" s="1">
-        <v>0</v>
-      </c>
-      <c r="G78" s="1">
+      <c r="G78" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="H78" s="1">
+        <v>1</v>
+      </c>
+      <c r="J78" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C79" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G79" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="E79" s="1">
-        <v>0</v>
-      </c>
-      <c r="G79" s="1">
+      <c r="H79" s="1">
+        <v>1</v>
+      </c>
+      <c r="J79" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E80" s="1">
-        <v>0</v>
-      </c>
-      <c r="J80" s="1">
+        <v>308</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H80" s="1">
+        <v>0</v>
+      </c>
+      <c r="M80" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E81" s="1">
-        <v>0</v>
-      </c>
-      <c r="I81" s="1">
+      <c r="G81" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H81" s="1">
+        <v>0</v>
+      </c>
+      <c r="L81" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E82" s="1">
-        <v>0</v>
+        <v>312</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="H82" s="1">
+        <v>0</v>
+      </c>
+      <c r="K82" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="E83" s="1">
-        <v>0</v>
+        <v>314</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="H83" s="1">
-        <v>1</v>
-      </c>
-      <c r="I83" s="1">
-        <v>1</v>
-      </c>
-      <c r="J83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K83" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L83" s="1">
+        <v>1</v>
+      </c>
+      <c r="M83" s="1">
+        <v>1</v>
+      </c>
+      <c r="N83" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="G84" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="E84" s="1">
-        <v>1</v>
-      </c>
       <c r="H84" s="1">
-        <v>2</v>
-      </c>
-      <c r="I84" s="1">
-        <v>2</v>
-      </c>
-      <c r="J84" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K84" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L84" s="1">
+        <v>2</v>
+      </c>
+      <c r="M84" s="1">
+        <v>2</v>
+      </c>
+      <c r="N84" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="E85" s="1">
-        <v>2</v>
+        <v>319</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="H85" s="1">
-        <v>3</v>
-      </c>
-      <c r="I85" s="1">
-        <v>3</v>
-      </c>
-      <c r="J85" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K85" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L85" s="1">
+        <v>3</v>
+      </c>
+      <c r="M85" s="1">
+        <v>3</v>
+      </c>
+      <c r="N85" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E86" s="1">
-        <v>0</v>
-      </c>
-      <c r="F86" s="1">
+        <v>324</v>
+      </c>
+      <c r="H86" s="1">
+        <v>0</v>
+      </c>
+      <c r="I86" s="1">
         <v>-2</v>
       </c>
-      <c r="G86" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J86" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="E87" s="1">
-        <v>1</v>
-      </c>
-      <c r="F87" s="1">
+        <v>325</v>
+      </c>
+      <c r="H87" s="1">
+        <v>1</v>
+      </c>
+      <c r="I87" s="1">
         <v>-3</v>
       </c>
-      <c r="G87" s="1">
+      <c r="J87" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="E88" s="1">
-        <v>0</v>
-      </c>
-      <c r="F88" s="1">
+        <v>322</v>
+      </c>
+      <c r="H88" s="1">
+        <v>0</v>
+      </c>
+      <c r="I88" s="1">
         <v>-10</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C89" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G89" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D89" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="E89" s="1">
-        <v>0</v>
-      </c>
-      <c r="G89" s="1">
+      <c r="H89" s="1">
+        <v>1</v>
+      </c>
+      <c r="J89" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B90" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C90" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="E90" s="1">
-        <v>0</v>
-      </c>
-      <c r="I90" s="1">
+      <c r="G90" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="H90" s="1">
+        <v>0</v>
+      </c>
+      <c r="L90" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B91" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="E91" s="1">
-        <v>0</v>
-      </c>
-      <c r="J91" s="1">
+      <c r="G91" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="H91" s="1">
+        <v>0</v>
+      </c>
+      <c r="M91" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C92" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G92" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="D92" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="E92" s="1">
-        <v>0</v>
-      </c>
-      <c r="G92" s="1">
-        <v>1</v>
-      </c>
       <c r="H92" s="1">
-        <v>1</v>
-      </c>
-      <c r="I92" s="1">
+        <v>0</v>
+      </c>
+      <c r="J92" s="1">
         <v>1</v>
       </c>
       <c r="K92" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L92" s="1">
+        <v>1</v>
+      </c>
+      <c r="N92" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="E93" s="1">
-        <v>1</v>
-      </c>
-      <c r="G93" s="1">
-        <v>2</v>
+        <v>340</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="H93" s="1">
-        <v>2</v>
-      </c>
-      <c r="I93" s="1">
+        <v>1</v>
+      </c>
+      <c r="J93" s="1">
         <v>2</v>
       </c>
       <c r="K93" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L93" s="1">
+        <v>2</v>
+      </c>
+      <c r="N93" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B94" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="G94" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="D94" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="E94" s="1">
-        <v>0</v>
-      </c>
-      <c r="G94" s="1">
-        <v>1</v>
-      </c>
       <c r="H94" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J94" s="1">
         <v>1</v>
@@ -3645,224 +3794,221 @@
       <c r="K94" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M94" s="1">
+        <v>1</v>
+      </c>
+      <c r="N94" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="E95" s="1">
-        <v>0</v>
-      </c>
-      <c r="I95" s="1">
+        <v>345</v>
+      </c>
+      <c r="H95" s="1">
+        <v>0</v>
+      </c>
+      <c r="L95" s="1">
         <v>-2</v>
       </c>
-      <c r="K95" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N95" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="E96" s="1">
-        <v>0</v>
-      </c>
-      <c r="I96" s="1">
+        <v>346</v>
+      </c>
+      <c r="H96" s="1">
+        <v>0</v>
+      </c>
+      <c r="L96" s="1">
         <v>-1</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="G97" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="E97" s="1">
-        <v>0</v>
-      </c>
-      <c r="G97" s="1">
-        <v>1</v>
-      </c>
-      <c r="I97" s="1">
-        <v>1</v>
+      <c r="H97" s="1">
+        <v>0</v>
       </c>
       <c r="J97" s="1">
         <v>1</v>
       </c>
-      <c r="K97" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L97" s="1">
+        <v>1</v>
+      </c>
+      <c r="M97" s="1">
+        <v>1</v>
+      </c>
+      <c r="N97" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="E98" s="1">
-        <v>0</v>
+        <v>350</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>353</v>
       </c>
       <c r="H98" s="1">
-        <v>1</v>
-      </c>
-      <c r="I98" s="1">
-        <v>1</v>
-      </c>
-      <c r="J98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K98" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L98" s="1">
+        <v>1</v>
+      </c>
+      <c r="M98" s="1">
+        <v>1</v>
+      </c>
+      <c r="N98" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C99" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="G99" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="D99" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="E99" s="1">
-        <v>1</v>
-      </c>
       <c r="H99" s="1">
-        <v>2</v>
-      </c>
-      <c r="I99" s="1">
-        <v>2</v>
-      </c>
-      <c r="J99" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K99" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L99" s="1">
+        <v>2</v>
+      </c>
+      <c r="M99" s="1">
+        <v>2</v>
+      </c>
+      <c r="N99" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C100" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="G100" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="D100" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="E100" s="1">
-        <v>1</v>
-      </c>
-      <c r="G100" s="1">
-        <v>2</v>
-      </c>
-      <c r="I100" s="1">
-        <v>2</v>
+      <c r="H100" s="1">
+        <v>1</v>
       </c>
       <c r="J100" s="1">
         <v>2</v>
       </c>
-      <c r="K100" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L100" s="1">
+        <v>2</v>
+      </c>
+      <c r="M100" s="1">
+        <v>2</v>
+      </c>
+      <c r="N100" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E101" s="1">
-        <v>0</v>
-      </c>
-      <c r="G101" s="1">
-        <v>2</v>
-      </c>
       <c r="H101" s="1">
+        <v>0</v>
+      </c>
+      <c r="J101" s="1">
+        <v>2</v>
+      </c>
+      <c r="K101" s="1">
         <v>-2</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="E102" s="1">
-        <v>0</v>
-      </c>
-      <c r="F102" s="1">
-        <v>1</v>
+      <c r="H102" s="1">
+        <v>0</v>
       </c>
       <c r="I102" s="1">
+        <v>1</v>
+      </c>
+      <c r="L102" s="1">
         <v>-2</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C103" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="G103" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="D103" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="E103" s="1">
-        <v>0</v>
-      </c>
-      <c r="G103" s="1">
-        <v>1</v>
-      </c>
       <c r="H103" s="1">
-        <v>1</v>
-      </c>
-      <c r="I103" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J103" s="1">
         <v>1</v>
@@ -3870,31 +4016,31 @@
       <c r="K103" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L103" s="1">
+        <v>1</v>
+      </c>
+      <c r="M103" s="1">
+        <v>1</v>
+      </c>
+      <c r="N103" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="D104" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="E104" s="1">
-        <v>1</v>
-      </c>
-      <c r="G104" s="1">
-        <v>2</v>
+      <c r="G104" s="5" t="s">
+        <v>366</v>
       </c>
       <c r="H104" s="1">
-        <v>2</v>
-      </c>
-      <c r="I104" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J104" s="1">
         <v>2</v>
@@ -3902,128 +4048,191 @@
       <c r="K104" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L104" s="1">
+        <v>2</v>
+      </c>
+      <c r="M104" s="1">
+        <v>2</v>
+      </c>
+      <c r="N104" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C105" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="G105" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="D105" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="E105" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H105" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C106" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="G106" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="D106" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="E106" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H106" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="E107" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="H107" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B108" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="E108" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H108" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="H109" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="H110" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="H111" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="H112" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="H113" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="H114" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="120" spans="1:1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>132</v>
       </c>

</xml_diff>